<commit_message>
Files to test xlsx run tool
</commit_message>
<xml_diff>
--- a/test/resources/evaluation/xlsx_files/test_sorted_order.xlsx
+++ b/test/resources/evaluation/xlsx_files/test_sorted_order.xlsx
@@ -4,6 +4,8 @@
   <workbookPr/>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="inspection_results1" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="inspection_results2" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="Z_0FE3D27A_F353_4CEC_BF1C_74962B9116E8_.wvu.FilterData" localSheetId="0" hidden="1">Sheet1!$C$1:$C$998</definedName>
@@ -975,4 +977,1172 @@
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="7" t="inlineStr">
+        <is>
+          <t>language</t>
+        </is>
+      </c>
+      <c r="B1" s="7" t="inlineStr">
+        <is>
+          <t>code</t>
+        </is>
+      </c>
+      <c r="C1" s="7" t="inlineStr">
+        <is>
+          <t>grade</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0" t="inlineStr">
+        <is>
+          <t>java11</t>
+        </is>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">public class Main {
+    public static void main(String[] args) {
+        int variable = 123456;  // Change this line
+        System.out.println(variable);
+    }
+}
+</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">{"quality": {"code": "EXCELLENT", "text": "Code quality (beta): EXCELLENT"}, "issues": [{"code": "Code Style", "text": "Number 123456 should separate every third digit with an underscore", "line": "int variable = 123456;  // Change this line", "line_number": 4, "column_number": 1, "category": "BEST_PRACTICES"}]}
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="inlineStr">
+        <is>
+          <t>java11</t>
+        </is>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">class Main {
+    public static void main(String[] args) {
+        System.out.println(0);
+        System.out.println(1);
+        System.out.println(2);
+                System.out.println(3);
+                        System.out.println(4);
+    }
+}
+</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">{"quality": {"code": "MODERATE", "text": "Code quality (beta): MODERATE"}, "issues": [{"code": "IndentationCheck", "text": "'method def' child has incorrect indentation level 16, expected level should be 8.", "line": "System.out.println(3);", "line_number": 6, "column_number": 1, "category": "CODE_STYLE"}, {"code": "IndentationCheck", "text": "'method def' child has incorrect indentation level 24, expected level should be 8.", "line": "System.out.println(4);", "line_number": 7, "column_number": 1, "category": "CODE_STYLE"}]}
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="inlineStr">
+        <is>
+          <t>java11</t>
+        </is>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">class Main {
+    public static void main(String[] args) {
+        System.out.println("WE NEED TO");
+        System.out.println("");
+        System.out.println("LEARN JAVA");
+        System.out.println("");
+        System.out.println("AS QUICKLY AS POSSIBLE");
+    }
+}
+</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">{"quality": {"code": "EXCELLENT", "text": "Code quality (beta): EXCELLENT"}, "issues": []}
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="inlineStr">
+        <is>
+          <t>java8</t>
+        </is>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">import java.util.Arrays;
+import java.util.Scanner;
+public class Main {
+    private static class TableEntry&lt;T&gt; {
+        private final int key;
+        private final T value;
+        public TableEntry(int key, T value) {
+            this.key = key;
+            this.value = value;
+        }
+        public int getKey() {
+            return key;
+        }
+        public T getValue() {
+            return value;
+        }
+    }
+    private static class HashTable&lt;T&gt; {
+        private int size;
+        private TableEntry[] table;
+        public HashTable(int size) {
+            this.size = size;
+            table = new TableEntry[size];
+        }
+        public boolean put(int key, T value) {
+            int idx = findKey(key);
+            if (idx == -1) {
+                size *= 2;
+                table = Arrays.copyOf(table, size);
+                idx = findKey(key);
+            }
+            table[idx] = new TableEntry(key, value);
+            return true;
+        }
+        public T get(int key) {
+            int idx = findKey(key);
+            if (idx == -1 || table[idx] == null) {
+                return null;
+            }
+            return (T) table[idx].getValue();
+        }
+        private int findKey(int key) {
+            int hash = key % size;
+            while (!(table[hash] == null || table[hash].getKey() == key)) {
+                hash = (hash + 1) % size;
+                if (hash == key % size) {
+                    return -1;
+                }
+            }
+            return hash;
+        }
+        private void rehash() {
+            size *= 2;
+            TableEntry[] oldTable = table;
+            table = new TableEntry[size];
+            for (TableEntry tableEntry : oldTable) {
+                table[findKey(tableEntry.getKey())] = tableEntry;
+            }
+        }
+        @Override
+        public String toString() {
+            StringBuilder tableStringBuilder = new StringBuilder();
+            for (int i = 0; i &lt; table.length; i++) {
+                if (table[i] == null) {
+                    tableStringBuilder.append(i + ": null");
+                } else {
+                    tableStringBuilder.append(i + ": key=" + table[i].getKey()
+                            + ", value=" + table[i].getValue());
+                }
+                if (i &lt; table.length - 1) {
+                    tableStringBuilder.append("\n");
+                }
+            }
+            return tableStringBuilder.toString();
+        }
+    }
+    public static void main(String[] args) {
+        Scanner scanner = new Scanner(System.in);
+        int counter = scanner.nextInt();
+        HashTable&lt;String&gt; data = new HashTable&lt;&gt;(5);
+        while (counter != 0) {
+            data.put(scanner.nextInt(), scanner.next());
+            counter--;
+        }
+        System.out.println(data);
+    }
+}
+</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">{"quality": {"code": "EXCELLENT", "text": "Code quality (beta): EXCELLENT"}, "issues": []}
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="inlineStr">
+        <is>
+          <t>java8</t>
+        </is>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">import java.util.Arrays;
+import java.util.Scanner;
+public class Main {
+    private static class TableEntry&lt;T&gt; {
+        private final int key;
+        private final T value;
+        public TableEntry(int key, T value) {
+            this.key = key;
+            this.value = value;
+        }
+        public int getKey() {
+            return key;
+        }
+        public T getValue() {
+            return value;
+        }
+    }
+    private static class HashTable&lt;T&gt; {
+        private int size;
+        private TableEntry[] table;
+        public HashTable(int size) {
+            this.size = size;
+            table = new TableEntry[size];
+        }
+        public boolean put(int key, T value) {
+            int idx = findKey(key);
+            if (idx == -1) {
+                size *= 2;
+                table = Arrays.copyOf(table, size);
+                idx = findKey(key);
+            }
+            table[idx] = new TableEntry(key, value);
+            return true;
+        }
+        public T get(int key) {
+            int idx = findKey(key);
+            if (idx == -1 || table[idx] == null) {
+                return null;
+            }
+            return (T) table[idx].getValue();
+        }
+        public void remove(int key) {
+            table[findKey(key)] = null;
+        }
+        private int findKey(int key) {
+            int hash = key % size;
+            while (!(table[hash] == null || table[hash].getKey() == key)) {
+                hash = (hash + 1) % size;
+                if (hash == key % size) {
+                    return -1;
+                }
+            }
+            return hash;
+        }
+        private void rehash() {
+            size *= 2;
+            TableEntry[] oldTable = table;
+            table = new TableEntry[size];
+            for (TableEntry tableEntry : oldTable) {
+                table[findKey(tableEntry.getKey())] = tableEntry;
+            }
+        }
+        @Override
+        public String toString() {
+            StringBuilder tableStringBuilder = new StringBuilder();
+            for (int i = 0; i &lt; table.length; i++) {
+                if (table[i] == null) {
+                    tableStringBuilder.append(i + ": null");
+                } else {
+                    tableStringBuilder.append(i + ": key=" + table[i].getKey()
+                            + ", value=" + table[i].getValue());
+                }
+                if (i &lt; table.length - 1) {
+                    tableStringBuilder.append("\n");
+                }
+            }
+            return tableStringBuilder.toString();
+        }
+    }
+    public static void main(String[] args) {
+        Scanner scanner = new Scanner(System.in);
+        int counter = scanner.nextInt();
+        HashTable&lt;String&gt; data = new HashTable&lt;&gt;(counter);
+        while (counter != 0) {
+            String command = scanner.next();
+            switch (command) {
+                case "put":
+                    data.put(scanner.nextInt(), scanner.next());
+                    break;
+                case "get":
+                    String  val = data.get(scanner.nextInt());
+                    System.out.println(val == null ? - 1: val);
+                    break;
+                case "remove":
+                    data.remove(scanner.nextInt());
+                    break;
+            }
+            counter--;
+        }
+    }
+}
+</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">{"quality": {"code": "BAD", "text": "Code quality (beta): BAD"}, "issues": [{"code": "MissingSwitchDefaultCheck", "text": "switch without \"default\" clause.", "line": "switch (command) {", "line_number": 112, "column_number": 1, "category": "ERROR_PRONE"}, {"code": "NoWhitespaceAfterCheck", "text": "'-' is followed by whitespace.", "line": "System.out.println(val == null ? - 1: val);", "line_number": 118, "column_number": 54, "category": "CODE_STYLE"}, {"code": "WhitespaceAroundCheck", "text": "':' is not preceded with whitespace.", "line": "System.out.println(val == null ? - 1: val);", "line_number": 118, "column_number": 57, "category": "CODE_STYLE"}]}
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="inlineStr">
+        <is>
+          <t>java8</t>
+        </is>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">import java.util.Scanner;
+public class Main {
+    private static class TableEntry&lt;T&gt; {
+        private final int key;
+        private final T value;
+        private boolean removed;
+        public TableEntry(int key, T value) {
+            this.key = key;
+            this.value = value;
+        }
+        public int getKey() {
+            return key;
+        }
+        public T getValue() {
+            return value;
+        }
+        public void remove() {
+             removed = true;   
+        }
+        public boolean isRemoved() {
+             return removed;   
+        }
+    }
+    private static class HashTable&lt;T&gt; {
+        private int size;
+        private TableEntry[] table;
+        public HashTable(int size) {
+            this.size = size;
+            table = new TableEntry[size];
+        }
+        public boolean put(int key, T value) {
+            int idx = findKey(key);
+            if (idx == -1) {
+                return false;
+            }
+            table[idx] = new TableEntry(key, value);
+            return true;
+        }
+        public T get(int key) {
+            int idx = findKey(key);
+            if (idx == -1 || table[idx] == null || table[idx].isRemoved()) {
+                return null;
+            }
+            return (T) table[idx].getValue();
+        }
+        public void remove(int key) {
+            int idx = findKey(key);
+            if (idx != -1 &amp;&amp; table[idx] != null) {
+                table[idx].remove();
+            }
+        }
+        private int findKey(int key) {
+            int hash = key % size;
+            while (table[hash] != null &amp;&amp; table[hash].getKey() != key) {
+                hash = (hash + 1) % size;
+                if (hash == key % size) {
+                    return -1;
+                }
+            }
+            return hash;
+        }
+        private void rehash() {
+            // put your code here
+        }
+    }
+    public static void main(String[] args) {
+        // put your code here
+        Scanner sc = new Scanner(System.in);
+        HashTable&lt;String&gt; ht = new HashTable(10000);
+        int n = sc.nextInt();
+        while (n-- &gt; 0) {
+            String command = sc.next();
+            if ("put".equals(command)) {
+                ht.put(sc.nextInt(), sc.next());
+            } else if ("get".equals(command)) {
+                String s = ht.get(sc.nextInt());
+                System.out.println(s == null ? "-1" : s);
+            } else if ("remove".equals(command)) {
+                ht.remove(sc.nextInt());
+            }
+        }
+    }
+}
+</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">{"quality": {"code": "GOOD", "text": "Code quality (beta): GOOD"}, "issues": [{"code": "IndentationCheck", "text": "'method def' child has incorrect indentation level 13, expected level should be 12.", "line": "removed = true;", "line_number": 23, "column_number": 1, "category": "CODE_STYLE"}, {"code": "IndentationCheck", "text": "'method def' child has incorrect indentation level 13, expected level should be 12.", "line": "return removed;", "line_number": 27, "column_number": 1, "category": "CODE_STYLE"}, {"code": "Code Style", "text": "Number 10000 should separate every third digit with an underscore", "line": "HashTable&lt;String&gt; ht = new HashTable(10000);", "line_number": 90, "column_number": 1, "category": "BEST_PRACTICES"}]}
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="inlineStr">
+        <is>
+          <t>kotlin</t>
+        </is>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">import java.util.*;
+fun main(args: Array&lt;String&gt;) {
+    val scanner = Scanner(System.`in`)
+    // put your code here
+    val sq = scanner.nextDouble()
+    val sqrt = Math.sqrt(Math.sqrt(sq))
+    println(sqrt)
+}
+</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">{"quality": {"code": "GOOD", "text": "Code quality (beta): GOOD"}, "issues": [{"code": "NoSemicolons", "text": "Unnecessary semicolon", "line": "import java.util.*;", "line_number": 1, "column_number": 19, "category": "CODE_STYLE"}]}
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="inlineStr">
+        <is>
+          <t>kotlin</t>
+        </is>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">fun main() {
+    TODO("Write some code to cause an exception")
+    print(3/0)
+}
+</t>
+        </is>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">{"quality": {"code": "GOOD", "text": "Code quality (beta): GOOD"}, "issues": [{"code": "SpacingAroundOperators", "text": "Missing spacing around \"/\"", "line": "print(3/0)", "line_number": 3, "column_number": 12, "category": "CODE_STYLE"}]}
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="inlineStr">
+        <is>
+          <t>kotlin</t>
+        </is>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">import java.util.*
+fun main(args: Array&lt;String&gt;) {
+    val scanner = Scanner(System.`in`)
+    // put your code here
+    val line = scanner.nextLine()
+    // val num = 0
+    repeat(10){
+        println(line)
+    }
+}
+</t>
+        </is>
+      </c>
+      <c r="C10" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">{"quality": {"code": "GOOD", "text": "Code quality (beta): GOOD"}, "issues": [{"code": "SpacingAroundCurly", "text": "Missing spacing before \"{\"", "line": "repeat(10){", "line_number": 8, "column_number": 15, "category": "CODE_STYLE"}]}
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="inlineStr">
+        <is>
+          <t>python3</t>
+        </is>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">random_numbers = ['1', '22', '333', '4444', '55555']
+print("\n".join(random_numbers))
+</t>
+        </is>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">{"quality": {"code": "EXCELLENT", "text": "Code quality (beta): EXCELLENT"}, "issues": []}
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="inlineStr">
+        <is>
+          <t>python3</t>
+        </is>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">s = "Hello"
+</t>
+        </is>
+      </c>
+      <c r="C12" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">{"quality": {"code": "EXCELLENT", "text": "Code quality (beta): EXCELLENT"}, "issues": []}
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="inlineStr">
+        <is>
+          <t>python3</t>
+        </is>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">text = input()
+words = text.split()
+for word in words:
+    # finish the code here
+    if word.startswith("WWW."):
+        print(word)
+    elif word.startswith("www."):
+        print(word)
+    elif word.startswith("https://"):
+        print(word)
+    elif word.startswith("HTTPS://"):
+        print(word)
+    elif word.startswith("http://"):
+        print(word)
+    elif word.startswith("HTTP://"):
+        print(word)
+    else:
+        continue
+</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">{"quality": {"code": "EXCELLENT", "text": "Code quality (beta): EXCELLENT"}, "issues": [{"code": "WPS327", "text": "Found useless `continue` at the end of the loop", "line": "for word in words:", "line_number": 3, "column_number": 1, "category": "BEST_PRACTICES"}, {"code": "WPS223", "text": "Found too many `elif` branches: 5 &gt; 3", "line": "if word.startswith(\"WWW.\"):", "line_number": 5, "column_number": 5, "category": "COMPLEXITY"}]}
+</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="7" t="inlineStr">
+        <is>
+          <t>language</t>
+        </is>
+      </c>
+      <c r="B1" s="7" t="inlineStr">
+        <is>
+          <t>code</t>
+        </is>
+      </c>
+      <c r="C1" s="7" t="inlineStr">
+        <is>
+          <t>grade</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0" t="inlineStr">
+        <is>
+          <t>java11</t>
+        </is>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">public class Main {
+    public static void main(String[] args) {
+        int variable = 123456;  // Change this line
+        System.out.println(variable);
+    }
+}
+</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>EXCELLENT</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="inlineStr">
+        <is>
+          <t>java11</t>
+        </is>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">class Main {
+    public static void main(String[] args) {
+        System.out.println(0);
+        System.out.println(1);
+        System.out.println(2);
+                System.out.println(3);
+                        System.out.println(4);
+    }
+}
+</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>MODERATE</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="inlineStr">
+        <is>
+          <t>java11</t>
+        </is>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">class Main {
+    public static void main(String[] args) {
+        System.out.println("WE NEED TO");
+        System.out.println("");
+        System.out.println("LEARN JAVA");
+        System.out.println("");
+        System.out.println("AS QUICKLY AS POSSIBLE");
+    }
+}
+</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>EXCELLENT</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="inlineStr">
+        <is>
+          <t>java8</t>
+        </is>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">import java.util.Arrays;
+import java.util.Scanner;
+public class Main {
+    private static class TableEntry&lt;T&gt; {
+        private final int key;
+        private final T value;
+        public TableEntry(int key, T value) {
+            this.key = key;
+            this.value = value;
+        }
+        public int getKey() {
+            return key;
+        }
+        public T getValue() {
+            return value;
+        }
+    }
+    private static class HashTable&lt;T&gt; {
+        private int size;
+        private TableEntry[] table;
+        public HashTable(int size) {
+            this.size = size;
+            table = new TableEntry[size];
+        }
+        public boolean put(int key, T value) {
+            int idx = findKey(key);
+            if (idx == -1) {
+                size *= 2;
+                table = Arrays.copyOf(table, size);
+                idx = findKey(key);
+            }
+            table[idx] = new TableEntry(key, value);
+            return true;
+        }
+        public T get(int key) {
+            int idx = findKey(key);
+            if (idx == -1 || table[idx] == null) {
+                return null;
+            }
+            return (T) table[idx].getValue();
+        }
+        private int findKey(int key) {
+            int hash = key % size;
+            while (!(table[hash] == null || table[hash].getKey() == key)) {
+                hash = (hash + 1) % size;
+                if (hash == key % size) {
+                    return -1;
+                }
+            }
+            return hash;
+        }
+        private void rehash() {
+            size *= 2;
+            TableEntry[] oldTable = table;
+            table = new TableEntry[size];
+            for (TableEntry tableEntry : oldTable) {
+                table[findKey(tableEntry.getKey())] = tableEntry;
+            }
+        }
+        @Override
+        public String toString() {
+            StringBuilder tableStringBuilder = new StringBuilder();
+            for (int i = 0; i &lt; table.length; i++) {
+                if (table[i] == null) {
+                    tableStringBuilder.append(i + ": null");
+                } else {
+                    tableStringBuilder.append(i + ": key=" + table[i].getKey()
+                            + ", value=" + table[i].getValue());
+                }
+                if (i &lt; table.length - 1) {
+                    tableStringBuilder.append("\n");
+                }
+            }
+            return tableStringBuilder.toString();
+        }
+    }
+    public static void main(String[] args) {
+        Scanner scanner = new Scanner(System.in);
+        int counter = scanner.nextInt();
+        HashTable&lt;String&gt; data = new HashTable&lt;&gt;(5);
+        while (counter != 0) {
+            data.put(scanner.nextInt(), scanner.next());
+            counter--;
+        }
+        System.out.println(data);
+    }
+}
+</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>EXCELLENT</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="inlineStr">
+        <is>
+          <t>java8</t>
+        </is>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">import java.util.Arrays;
+import java.util.Scanner;
+public class Main {
+    private static class TableEntry&lt;T&gt; {
+        private final int key;
+        private final T value;
+        public TableEntry(int key, T value) {
+            this.key = key;
+            this.value = value;
+        }
+        public int getKey() {
+            return key;
+        }
+        public T getValue() {
+            return value;
+        }
+    }
+    private static class HashTable&lt;T&gt; {
+        private int size;
+        private TableEntry[] table;
+        public HashTable(int size) {
+            this.size = size;
+            table = new TableEntry[size];
+        }
+        public boolean put(int key, T value) {
+            int idx = findKey(key);
+            if (idx == -1) {
+                size *= 2;
+                table = Arrays.copyOf(table, size);
+                idx = findKey(key);
+            }
+            table[idx] = new TableEntry(key, value);
+            return true;
+        }
+        public T get(int key) {
+            int idx = findKey(key);
+            if (idx == -1 || table[idx] == null) {
+                return null;
+            }
+            return (T) table[idx].getValue();
+        }
+        public void remove(int key) {
+            table[findKey(key)] = null;
+        }
+        private int findKey(int key) {
+            int hash = key % size;
+            while (!(table[hash] == null || table[hash].getKey() == key)) {
+                hash = (hash + 1) % size;
+                if (hash == key % size) {
+                    return -1;
+                }
+            }
+            return hash;
+        }
+        private void rehash() {
+            size *= 2;
+            TableEntry[] oldTable = table;
+            table = new TableEntry[size];
+            for (TableEntry tableEntry : oldTable) {
+                table[findKey(tableEntry.getKey())] = tableEntry;
+            }
+        }
+        @Override
+        public String toString() {
+            StringBuilder tableStringBuilder = new StringBuilder();
+            for (int i = 0; i &lt; table.length; i++) {
+                if (table[i] == null) {
+                    tableStringBuilder.append(i + ": null");
+                } else {
+                    tableStringBuilder.append(i + ": key=" + table[i].getKey()
+                            + ", value=" + table[i].getValue());
+                }
+                if (i &lt; table.length - 1) {
+                    tableStringBuilder.append("\n");
+                }
+            }
+            return tableStringBuilder.toString();
+        }
+    }
+    public static void main(String[] args) {
+        Scanner scanner = new Scanner(System.in);
+        int counter = scanner.nextInt();
+        HashTable&lt;String&gt; data = new HashTable&lt;&gt;(counter);
+        while (counter != 0) {
+            String command = scanner.next();
+            switch (command) {
+                case "put":
+                    data.put(scanner.nextInt(), scanner.next());
+                    break;
+                case "get":
+                    String  val = data.get(scanner.nextInt());
+                    System.out.println(val == null ? - 1: val);
+                    break;
+                case "remove":
+                    data.remove(scanner.nextInt());
+                    break;
+            }
+            counter--;
+        }
+    }
+}
+</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>BAD</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="inlineStr">
+        <is>
+          <t>java8</t>
+        </is>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">import java.util.Scanner;
+public class Main {
+    private static class TableEntry&lt;T&gt; {
+        private final int key;
+        private final T value;
+        private boolean removed;
+        public TableEntry(int key, T value) {
+            this.key = key;
+            this.value = value;
+        }
+        public int getKey() {
+            return key;
+        }
+        public T getValue() {
+            return value;
+        }
+        public void remove() {
+             removed = true;   
+        }
+        public boolean isRemoved() {
+             return removed;   
+        }
+    }
+    private static class HashTable&lt;T&gt; {
+        private int size;
+        private TableEntry[] table;
+        public HashTable(int size) {
+            this.size = size;
+            table = new TableEntry[size];
+        }
+        public boolean put(int key, T value) {
+            int idx = findKey(key);
+            if (idx == -1) {
+                return false;
+            }
+            table[idx] = new TableEntry(key, value);
+            return true;
+        }
+        public T get(int key) {
+            int idx = findKey(key);
+            if (idx == -1 || table[idx] == null || table[idx].isRemoved()) {
+                return null;
+            }
+            return (T) table[idx].getValue();
+        }
+        public void remove(int key) {
+            int idx = findKey(key);
+            if (idx != -1 &amp;&amp; table[idx] != null) {
+                table[idx].remove();
+            }
+        }
+        private int findKey(int key) {
+            int hash = key % size;
+            while (table[hash] != null &amp;&amp; table[hash].getKey() != key) {
+                hash = (hash + 1) % size;
+                if (hash == key % size) {
+                    return -1;
+                }
+            }
+            return hash;
+        }
+        private void rehash() {
+            // put your code here
+        }
+    }
+    public static void main(String[] args) {
+        // put your code here
+        Scanner sc = new Scanner(System.in);
+        HashTable&lt;String&gt; ht = new HashTable(10000);
+        int n = sc.nextInt();
+        while (n-- &gt; 0) {
+            String command = sc.next();
+            if ("put".equals(command)) {
+                ht.put(sc.nextInt(), sc.next());
+            } else if ("get".equals(command)) {
+                String s = ht.get(sc.nextInt());
+                System.out.println(s == null ? "-1" : s);
+            } else if ("remove".equals(command)) {
+                ht.remove(sc.nextInt());
+            }
+        }
+    }
+}
+</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>GOOD</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="inlineStr">
+        <is>
+          <t>kotlin</t>
+        </is>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">import java.util.*;
+fun main(args: Array&lt;String&gt;) {
+    val scanner = Scanner(System.`in`)
+    // put your code here
+    val sq = scanner.nextDouble()
+    val sqrt = Math.sqrt(Math.sqrt(sq))
+    println(sqrt)
+}
+</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>GOOD</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="inlineStr">
+        <is>
+          <t>kotlin</t>
+        </is>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">fun main() {
+    TODO("Write some code to cause an exception")
+    print(3/0)
+}
+</t>
+        </is>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>GOOD</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="inlineStr">
+        <is>
+          <t>kotlin</t>
+        </is>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">import java.util.*
+fun main(args: Array&lt;String&gt;) {
+    val scanner = Scanner(System.`in`)
+    // put your code here
+    val line = scanner.nextLine()
+    // val num = 0
+    repeat(10){
+        println(line)
+    }
+}
+</t>
+        </is>
+      </c>
+      <c r="C10" s="0" t="inlineStr">
+        <is>
+          <t>GOOD</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="inlineStr">
+        <is>
+          <t>python3</t>
+        </is>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">random_numbers = ['1', '22', '333', '4444', '55555']
+print("\n".join(random_numbers))
+</t>
+        </is>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>EXCELLENT</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="inlineStr">
+        <is>
+          <t>python3</t>
+        </is>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">s = "Hello"
+</t>
+        </is>
+      </c>
+      <c r="C12" s="0" t="inlineStr">
+        <is>
+          <t>EXCELLENT</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="inlineStr">
+        <is>
+          <t>python3</t>
+        </is>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">text = input()
+words = text.split()
+for word in words:
+    # finish the code here
+    if word.startswith("WWW."):
+        print(word)
+    elif word.startswith("www."):
+        print(word)
+    elif word.startswith("https://"):
+        print(word)
+    elif word.startswith("HTTPS://"):
+        print(word)
+    elif word.startswith("http://"):
+        print(word)
+    elif word.startswith("HTTP://"):
+        print(word)
+    else:
+        continue
+</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>EXCELLENT</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>